<commit_message>
Arreglo de importar excel y botones en crear producto
</commit_message>
<xml_diff>
--- a/componentes/formato_productos.xlsx
+++ b/componentes/formato_productos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto SIMR\componentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B53D7D-C0BE-41B9-B208-1B4AAB45CCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79788DD-CD89-47D8-8C2C-003C23C4C98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -55,13 +55,13 @@
     <t>marca</t>
   </si>
   <si>
-    <t>unidadmedida</t>
-  </si>
-  <si>
     <t>ubicacion</t>
   </si>
   <si>
     <t>proveedor</t>
+  </si>
+  <si>
+    <t>clase</t>
   </si>
 </sst>
 </file>
@@ -411,14 +411,15 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -458,13 +459,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglo error correo vacio y css
</commit_message>
<xml_diff>
--- a/componentes/formato_productos.xlsx
+++ b/componentes/formato_productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto SIMR\componentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79788DD-CD89-47D8-8C2C-003C23C4C98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30314F22-8B86-452E-8CAE-62E7B6C1627C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24810" yWindow="3435" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>codigo1</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>cantidad</t>
-  </si>
-  <si>
-    <t>descripcion</t>
   </si>
   <si>
     <t>categoria</t>
@@ -408,23 +405,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,16 +452,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>